<commit_message>
Updated Reading Data From Excel and Implemented Random access
</commit_message>
<xml_diff>
--- a/FlipkartTest/src/main/resources/TestData/FlipkartTestData.xlsx
+++ b/FlipkartTest/src/main/resources/TestData/FlipkartTestData.xlsx
@@ -3,16 +3,16 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{157D796F-1BFA-4414-80DA-98064D33C985}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{C89D8F20-A5C1-45FD-8A82-898B4763B4EB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1152" yWindow="1152" windowWidth="23304" windowHeight="13224" activeTab="1" xr2:uid="{0D5715A3-F87A-499B-AC13-B2E527F999EE}"/>
+    <workbookView xWindow="384" yWindow="384" windowWidth="23304" windowHeight="13224" activeTab="1" xr2:uid="{0D5715A3-F87A-499B-AC13-B2E527F999EE}"/>
   </bookViews>
   <sheets>
     <sheet name="Credentials" sheetId="1" r:id="rId1"/>
-    <sheet name="ApplicationDetails" sheetId="2" r:id="rId2"/>
+    <sheet name="AppDetails" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:R6"/>
+  <oleSize ref="A1:P13"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -93,9 +93,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -414,35 +415,36 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5546875" customWidth="1"/>
-    <col min="3" max="3" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="13.21875" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2">
+    <row r="2" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
         <v>7829892015</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
@@ -451,42 +453,46 @@
     <hyperlink ref="B2" r:id="rId1" xr:uid="{C51F3670-70FA-4786-B70B-97791715AEF8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C742F2B-D67F-48F9-959C-B6C4B8024A90}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12A5631B-8FF7-4C93-879C-E87FFEFA8F3F}">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.88671875" style="1"/>
+    <col min="2" max="2" width="25.5546875" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="2" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>8</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{29990C4C-F2E2-4025-BB5D-F08338C8050A}"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{98F2BC3C-D9D9-4580-B9C9-90150E2DA009}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>